<commit_message>
changed the analysis result files
</commit_message>
<xml_diff>
--- a/Overall Files/Analysis Result.xlsx
+++ b/Overall Files/Analysis Result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minsik/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minsik/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16BAB3FA-C47C-0C4C-84CE-386C9A55705E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90690E6-0861-5B4A-9EA3-4BB2C0CEFEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D191EDB1-F553-D84A-B803-B27A1F8FBA75}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{D191EDB1-F553-D84A-B803-B27A1F8FBA75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="553">
   <si>
     <t>Title</t>
   </si>
@@ -542,9 +542,6 @@
     <t>IEEE</t>
   </si>
   <si>
-    <t>NIPS</t>
-  </si>
-  <si>
     <t>medicine-nature-vision</t>
   </si>
   <si>
@@ -638,9 +635,6 @@
     <t>Matta, S.; Kumar, D.K.; Yu, Xinghuo; Burry, M.</t>
   </si>
   <si>
-    <t>IEEE Int. Conf. Signal Process</t>
-  </si>
-  <si>
     <t>Detection of obstructive sleep apnea through auditory display of heart rate variability</t>
   </si>
   <si>
@@ -656,9 +650,6 @@
     <t>Ma√ß√£s, Catarina; Martins, Pedro; Machado, Penousal</t>
   </si>
   <si>
-    <t>ICIV</t>
-  </si>
-  <si>
     <t>Ranking of Regional Blogs by Suitability for Sonification</t>
   </si>
   <si>
@@ -1695,6 +1686,15 @@
   </si>
   <si>
     <t>CardioSounds: A portable system to sonify ECG rhythm disturbances in real-time</t>
+  </si>
+  <si>
+    <t>ICONIP</t>
+  </si>
+  <si>
+    <t>ISCCSP</t>
+  </si>
+  <si>
+    <t>IV</t>
   </si>
 </sst>
 </file>
@@ -1743,10 +1743,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2061,10 +2062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78730E6-1DB0-FD44-93CC-339688788B9E}">
-  <dimension ref="A1:K200"/>
+  <dimension ref="A1:K201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3490,10 +3491,10 @@
         <v>167</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>34</v>
@@ -3509,10 +3510,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="C48" s="1">
         <v>2022</v>
@@ -3521,7 +3522,7 @@
         <v>167</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>74</v>
@@ -3540,10 +3541,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="C49" s="1">
         <v>2006</v>
@@ -3552,7 +3553,7 @@
         <v>167</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>74</v>
@@ -3573,10 +3574,10 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="C50" s="1">
         <v>2015</v>
@@ -3585,10 +3586,10 @@
         <v>167</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>34</v>
@@ -3604,10 +3605,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="C51" s="1">
         <v>2020</v>
@@ -3616,10 +3617,10 @@
         <v>167</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>34</v>
@@ -3635,10 +3636,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="C52" s="1">
         <v>2019</v>
@@ -3647,7 +3648,7 @@
         <v>167</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>33</v>
@@ -3666,10 +3667,10 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="C53" s="1">
         <v>2012</v>
@@ -3678,7 +3679,7 @@
         <v>167</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>33</v>
@@ -3697,10 +3698,10 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="C54" s="1">
         <v>2019</v>
@@ -3709,10 +3710,10 @@
         <v>167</v>
       </c>
       <c r="E54" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>34</v>
@@ -3728,10 +3729,10 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="C55" s="1">
         <v>2015</v>
@@ -3740,10 +3741,10 @@
         <v>167</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>34</v>
@@ -3759,10 +3760,10 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="C56" s="1">
         <v>2004</v>
@@ -3771,7 +3772,7 @@
         <v>167</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>200</v>
+        <v>551</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>93</v>
@@ -3790,10 +3791,10 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C57" s="1">
         <v>2000</v>
@@ -3802,7 +3803,7 @@
         <v>167</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>131</v>
@@ -3819,10 +3820,10 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C58" s="1">
         <v>2018</v>
@@ -3831,7 +3832,7 @@
         <v>167</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>206</v>
+        <v>552</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>93</v>
@@ -3848,10 +3849,10 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C59" s="1">
         <v>2006</v>
@@ -3860,7 +3861,7 @@
         <v>167</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>108</v>
@@ -3875,10 +3876,10 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C60" s="1">
         <v>2004</v>
@@ -3887,7 +3888,7 @@
         <v>167</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>81</v>
@@ -3906,10 +3907,10 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C61" s="1">
         <v>2003</v>
@@ -3918,10 +3919,10 @@
         <v>167</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>34</v>
@@ -3937,10 +3938,10 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C62" s="1">
         <v>2001</v>
@@ -3949,7 +3950,7 @@
         <v>167</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>81</v>
@@ -3968,7 +3969,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>104</v>
@@ -3977,13 +3978,13 @@
         <v>2021</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>34</v>
@@ -3999,19 +4000,19 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C64" s="1">
         <v>2008</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>74</v>
@@ -4032,19 +4033,19 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C65" s="1">
         <v>2022</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>44</v>
@@ -4063,19 +4064,19 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C66" s="1">
         <v>2017</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>20</v>
@@ -4084,7 +4085,7 @@
         <v>60</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I66" s="2"/>
       <c r="J66" s="1" t="s">
@@ -4094,19 +4095,19 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C67" s="1">
         <v>2023</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>141</v>
@@ -4127,22 +4128,22 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C68" s="1">
         <v>2008</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>34</v>
@@ -4156,19 +4157,19 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C69" s="1">
         <v>2021</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>86</v>
@@ -4177,7 +4178,7 @@
         <v>60</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I69" s="2"/>
       <c r="J69" s="1" t="s">
@@ -4187,22 +4188,22 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C70" s="1">
         <v>2021</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>34</v>
@@ -4218,19 +4219,19 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C71" s="1">
         <v>2014</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>93</v>
@@ -4239,7 +4240,7 @@
         <v>60</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
@@ -4247,22 +4248,22 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C72" s="1">
         <v>2016</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>34</v>
@@ -4278,19 +4279,19 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C73" s="1">
         <v>2010</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>141</v>
@@ -4309,22 +4310,22 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C74" s="1">
         <v>2008</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>40</v>
@@ -4336,19 +4337,19 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C75" s="1">
         <v>2011</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>93</v>
@@ -4367,19 +4368,19 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C76" s="1">
         <v>2009</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>93</v>
@@ -4396,19 +4397,19 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C77" s="1">
         <v>2017</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>48</v>
@@ -4427,19 +4428,19 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C78" s="1">
         <v>2011</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>74</v>
@@ -4460,19 +4461,19 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C79" s="1">
         <v>2018</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>48</v>
@@ -4489,19 +4490,19 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C80" s="1">
         <v>2019</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>93</v>
@@ -4520,19 +4521,19 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C81" s="1">
         <v>2016</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>48</v>
@@ -4549,19 +4550,19 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C82" s="1">
         <v>2017</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>39</v>
@@ -4578,19 +4579,19 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C83" s="1">
         <v>2020</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>108</v>
@@ -4607,19 +4608,19 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C84" s="1">
         <v>2022</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>48</v>
@@ -4638,19 +4639,19 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C85" s="1">
         <v>2023</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>74</v>
@@ -4659,7 +4660,7 @@
         <v>34</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I85" s="2"/>
       <c r="J85" s="1" t="s">
@@ -4669,22 +4670,22 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C86" s="1">
         <v>2008</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>40</v>
@@ -4698,22 +4699,22 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C87" s="1">
         <v>2017</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>34</v>
@@ -4731,22 +4732,22 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C88" s="1">
         <v>2016</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>34</v>
@@ -4762,22 +4763,22 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C89" s="1">
         <v>2019</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>40</v>
@@ -4789,19 +4790,19 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C90" s="1">
         <v>2002</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>108</v>
@@ -4820,19 +4821,19 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C91" s="1">
         <v>2021</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>81</v>
@@ -4842,24 +4843,26 @@
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
+      <c r="J91" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K91" s="2"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C92" s="1">
         <v>2016</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>81</v>
@@ -4878,19 +4881,19 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C93" s="1">
         <v>2013</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>81</v>
@@ -4909,19 +4912,19 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C94" s="1">
         <v>2000</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>81</v>
@@ -4936,19 +4939,19 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C95" s="1">
         <v>2013</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>81</v>
@@ -4967,22 +4970,22 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C96" s="1">
         <v>2012</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>40</v>
@@ -4996,19 +4999,19 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C97" s="1">
         <v>2009</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>74</v>
@@ -5023,19 +5026,19 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C98" s="1">
         <v>2012</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>81</v>
@@ -5050,19 +5053,19 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C99" s="1">
         <v>2004</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>74</v>
@@ -5071,7 +5074,7 @@
         <v>34</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
@@ -5079,19 +5082,19 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C100" s="1">
         <v>2016</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>20</v>
@@ -5100,7 +5103,7 @@
         <v>16</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>34</v>
@@ -5110,19 +5113,19 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C101" s="1">
         <v>2014</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>52</v>
@@ -5131,7 +5134,7 @@
         <v>34</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
@@ -5139,7 +5142,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>104</v>
@@ -5148,13 +5151,13 @@
         <v>2019</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>34</v>
@@ -5170,19 +5173,19 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C103" s="1">
         <v>2022</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>59</v>
@@ -5191,7 +5194,7 @@
         <v>34</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="I103" s="2"/>
       <c r="J103" s="1" t="s">
@@ -5201,19 +5204,19 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C104" s="1">
         <v>2005</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>108</v>
@@ -5225,27 +5228,29 @@
         <v>35</v>
       </c>
       <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
+      <c r="J104" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K104" s="2"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C105" s="1">
         <v>2018</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>40</v>
@@ -5259,19 +5264,19 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C106" s="1">
         <v>2019</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>81</v>
@@ -5280,7 +5285,7 @@
         <v>34</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I106" s="2"/>
       <c r="J106" s="1" t="s">
@@ -5290,19 +5295,19 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C107" s="1">
         <v>2008</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>141</v>
@@ -5319,22 +5324,22 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C108" s="1">
         <v>2015</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>34</v>
@@ -5350,19 +5355,19 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C109" s="1">
         <v>1997</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>39</v>
@@ -5383,19 +5388,19 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C110" s="1">
         <v>2018</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>81</v>
@@ -5404,7 +5409,7 @@
         <v>34</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="I110" s="2"/>
       <c r="J110" s="1" t="s">
@@ -5414,19 +5419,19 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C111" s="1">
         <v>2012</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>141</v>
@@ -5447,19 +5452,19 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C112" s="1">
         <v>2012</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>48</v>
@@ -5478,22 +5483,22 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C113" s="1">
         <v>2012</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
@@ -5505,19 +5510,19 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C114" s="1">
         <v>2018</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>44</v>
@@ -5536,19 +5541,19 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C115" s="1">
         <v>2020</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>52</v>
@@ -5567,19 +5572,19 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C116" s="1">
         <v>2013</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>44</v>
@@ -5594,19 +5599,19 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C117" s="1">
         <v>2019</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>81</v>
@@ -5615,7 +5620,7 @@
         <v>16</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="I117" s="2"/>
       <c r="J117" s="1" t="s">
@@ -5625,19 +5630,19 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C118" s="1">
         <v>2007</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>81</v>
@@ -5652,19 +5657,19 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C119" s="1">
         <v>2005</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>81</v>
@@ -5679,19 +5684,19 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C120" s="1">
         <v>2002</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>81</v>
@@ -5700,7 +5705,7 @@
         <v>60</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I120" s="2"/>
       <c r="J120" s="1" t="s">
@@ -5710,28 +5715,28 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C121" s="1">
         <v>2002</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I121" s="2"/>
       <c r="J121" s="2"/>
@@ -5739,19 +5744,19 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C122" s="1">
         <v>2007</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>81</v>
@@ -5760,7 +5765,7 @@
         <v>16</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="I122" s="2"/>
       <c r="J122" s="1" t="s">
@@ -5770,19 +5775,19 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C123" s="1">
         <v>2005</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>81</v>
@@ -5799,19 +5804,19 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C124" s="1">
         <v>2018</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>81</v>
@@ -5828,28 +5833,28 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C125" s="1">
         <v>2011</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I125" s="2"/>
       <c r="J125" s="1" t="s">
@@ -5859,19 +5864,19 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C126" s="1">
         <v>1997</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>81</v>
@@ -5888,19 +5893,19 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C127" s="1">
         <v>1996</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>93</v>
@@ -5919,19 +5924,19 @@
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C128" s="1">
         <v>2012</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>81</v>
@@ -5946,19 +5951,19 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C129" s="1">
         <v>2011</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>52</v>
@@ -5975,22 +5980,22 @@
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C130" s="1">
         <v>2006</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>34</v>
@@ -6004,19 +6009,19 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C131" s="1">
         <v>2008</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>81</v>
@@ -6025,7 +6030,7 @@
         <v>16</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="I131" s="2"/>
       <c r="J131" s="1" t="s">
@@ -6035,19 +6040,19 @@
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C132" s="1">
         <v>2012</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>151</v>
@@ -6056,7 +6061,7 @@
         <v>16</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="I132" s="2"/>
       <c r="J132" s="2"/>
@@ -6064,19 +6069,19 @@
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C133" s="1">
         <v>2018</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>93</v>
@@ -6085,7 +6090,7 @@
         <v>34</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I133" s="2"/>
       <c r="J133" s="2"/>
@@ -6093,19 +6098,19 @@
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C134" s="1">
         <v>2012</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>81</v>
@@ -6122,19 +6127,19 @@
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C135" s="1">
         <v>2014</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>81</v>
@@ -6153,19 +6158,19 @@
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C136" s="1">
         <v>2018</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>81</v>
@@ -6184,19 +6189,19 @@
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C137" s="1">
         <v>2013</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>48</v>
@@ -6213,7 +6218,7 @@
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>37</v>
@@ -6222,10 +6227,10 @@
         <v>2015</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>39</v>
@@ -6234,7 +6239,7 @@
         <v>60</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="I138" s="2"/>
       <c r="J138" s="1" t="s">
@@ -6244,19 +6249,19 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C139" s="1">
         <v>2008</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>81</v>
@@ -6265,7 +6270,7 @@
         <v>34</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I139" s="2"/>
       <c r="J139" s="1" t="s">
@@ -6275,19 +6280,19 @@
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C140" s="1">
         <v>2019</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>52</v>
@@ -6296,7 +6301,7 @@
         <v>34</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="I140" s="2"/>
       <c r="J140" s="1" t="s">
@@ -6306,28 +6311,28 @@
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C141" s="1">
         <v>2013</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="I141" s="2"/>
       <c r="J141" s="1" t="s">
@@ -6337,7 +6342,7 @@
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>160</v>
@@ -6346,13 +6351,13 @@
         <v>2021</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>34</v>
@@ -6366,19 +6371,19 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C143" s="1">
         <v>2017</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>86</v>
@@ -6393,19 +6398,19 @@
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C144" s="1">
         <v>2016</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F144" s="1" t="s">
         <v>33</v>
@@ -6424,19 +6429,19 @@
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C145" s="1">
         <v>2011</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>86</v>
@@ -6455,19 +6460,19 @@
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C146" s="1">
         <v>2011</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>33</v>
@@ -6484,19 +6489,19 @@
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C147" s="1">
         <v>2013</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>20</v>
@@ -6513,19 +6518,19 @@
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C148" s="1">
         <v>2001</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>93</v>
@@ -6542,19 +6547,19 @@
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C149" s="1">
         <v>2004</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>93</v>
@@ -6565,27 +6570,25 @@
       <c r="H149" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I149" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="I149" s="1"/>
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C150" s="1">
         <v>2018</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>81</v>
@@ -6600,28 +6603,28 @@
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C151" s="1">
         <v>2009</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G151" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="I151" s="2"/>
       <c r="J151" s="2"/>
@@ -6629,19 +6632,19 @@
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C152" s="1">
         <v>2019</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>108</v>
@@ -6660,19 +6663,19 @@
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C153" s="1">
         <v>2011</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>48</v>
@@ -6681,7 +6684,7 @@
         <v>34</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="I153" s="2"/>
       <c r="J153" s="2"/>
@@ -6689,19 +6692,19 @@
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C154" s="1">
         <v>2017</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>81</v>
@@ -6720,19 +6723,19 @@
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C155" s="1">
         <v>2008</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>141</v>
@@ -6753,19 +6756,19 @@
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C156" s="1">
         <v>2002</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>93</v>
@@ -6784,19 +6787,19 @@
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C157" s="1">
         <v>2009</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>48</v>
@@ -6811,19 +6814,19 @@
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C158" s="1">
         <v>2013</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>81</v>
@@ -6840,19 +6843,19 @@
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C159" s="1">
         <v>2004</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>81</v>
@@ -6871,19 +6874,19 @@
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C160" s="1">
         <v>2019</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>93</v>
@@ -6900,19 +6903,19 @@
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C161" s="1">
         <v>2021</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>33</v>
@@ -6921,7 +6924,7 @@
         <v>34</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="I161" s="2"/>
       <c r="J161" s="2"/>
@@ -6929,19 +6932,19 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C162" s="1">
         <v>2021</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>81</v>
@@ -6950,7 +6953,7 @@
         <v>34</v>
       </c>
       <c r="H162" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="I162" s="2"/>
       <c r="J162" s="1" t="s">
@@ -6960,19 +6963,19 @@
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C163" s="1">
         <v>2006</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>131</v>
@@ -6989,22 +6992,22 @@
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C164" s="1">
         <v>2019</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>60</v>
@@ -7022,28 +7025,28 @@
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C165" s="1">
         <v>2003</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G165" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I165" s="2"/>
       <c r="J165" s="1" t="s">
@@ -7053,22 +7056,22 @@
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C166" s="1">
         <v>2021</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G166" s="1" t="s">
         <v>40</v>
@@ -7082,19 +7085,19 @@
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C167" s="1">
         <v>2002</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>164</v>
@@ -7103,7 +7106,7 @@
         <v>34</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I167" s="2"/>
       <c r="J167" s="1" t="s">
@@ -7113,19 +7116,19 @@
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C168" s="1">
         <v>2018</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>33</v>
@@ -7146,19 +7149,19 @@
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C169" s="1">
         <v>2015</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>15</v>
@@ -7170,24 +7173,26 @@
         <v>17</v>
       </c>
       <c r="I169" s="2"/>
-      <c r="J169" s="2"/>
+      <c r="J169" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K169" s="2"/>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C170" s="1">
         <v>2017</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>33</v>
@@ -7206,19 +7211,19 @@
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C171" s="1">
         <v>2018</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>81</v>
@@ -7227,7 +7232,7 @@
         <v>34</v>
       </c>
       <c r="H171" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I171" s="2"/>
       <c r="J171" s="1" t="s">
@@ -7237,22 +7242,22 @@
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C172" s="1">
         <v>2004</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="G172" s="1" t="s">
         <v>40</v>
@@ -7266,28 +7271,28 @@
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C173" s="1">
         <v>2004</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="G173" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I173" s="2"/>
       <c r="J173" s="2"/>
@@ -7295,19 +7300,19 @@
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C174" s="1">
         <v>2015</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>81</v>
@@ -7324,19 +7329,19 @@
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C175" s="1">
         <v>2005</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>81</v>
@@ -7345,7 +7350,7 @@
         <v>34</v>
       </c>
       <c r="H175" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="I175" s="2"/>
       <c r="J175" s="1" t="s">
@@ -7355,19 +7360,19 @@
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C176" s="1">
         <v>2006</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>81</v>
@@ -7386,19 +7391,19 @@
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C177" s="1">
         <v>2019</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>93</v>
@@ -7417,22 +7422,22 @@
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C178" s="1">
         <v>2015</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G178" s="2"/>
       <c r="H178" s="2"/>
@@ -7444,19 +7449,19 @@
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C179" s="1">
         <v>1998</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>93</v>
@@ -7473,19 +7478,19 @@
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C180" s="1">
         <v>2012</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>81</v>
@@ -7502,19 +7507,19 @@
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C181" s="1">
         <v>1996</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>81</v>
@@ -7529,19 +7534,19 @@
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C182" s="1">
         <v>2021</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>131</v>
@@ -7560,19 +7565,19 @@
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C183" s="1">
         <v>2021</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>164</v>
@@ -7589,19 +7594,19 @@
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C184" s="1">
         <v>2014</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>93</v>
@@ -7613,27 +7618,31 @@
         <v>35</v>
       </c>
       <c r="I184" s="2"/>
-      <c r="J184" s="2"/>
-      <c r="K184" s="2"/>
+      <c r="J184" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K184" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C185" s="1">
         <v>2010</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="G185" s="1" t="s">
         <v>34</v>
@@ -7642,26 +7651,28 @@
         <v>35</v>
       </c>
       <c r="I185" s="2"/>
-      <c r="J185" s="2"/>
+      <c r="J185" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K185" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C186" s="1">
         <v>2021</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>81</v>
@@ -7678,19 +7689,19 @@
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C187" s="1">
         <v>2009</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>81</v>
@@ -7705,19 +7716,19 @@
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C188" s="1">
         <v>2007</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>81</v>
@@ -7734,19 +7745,19 @@
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C189" s="1">
         <v>2000</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>81</v>
@@ -7765,22 +7776,22 @@
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C190" s="1">
         <v>2021</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="G190" s="1" t="s">
         <v>34</v>
@@ -7796,22 +7807,22 @@
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C191" s="1">
         <v>2002</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G191" s="1" t="s">
         <v>70</v>
@@ -7827,19 +7838,19 @@
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C192" s="1">
         <v>2007</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>81</v>
@@ -7858,19 +7869,19 @@
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C193" s="1">
         <v>2001</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>93</v>
@@ -7889,22 +7900,22 @@
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C194" s="1">
         <v>2017</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G194" s="1" t="s">
         <v>34</v>
@@ -7920,22 +7931,22 @@
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C195" s="1">
         <v>2011</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="G195" s="1" t="s">
         <v>34</v>
@@ -7953,19 +7964,19 @@
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C196" s="1">
         <v>2018</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>81</v>
@@ -7984,22 +7995,22 @@
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C197" s="1">
         <v>2007</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G197" s="1" t="s">
         <v>34</v>
@@ -8013,19 +8024,19 @@
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C198" s="1">
         <v>2018</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>81</v>
@@ -8044,7 +8055,7 @@
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>95</v>
@@ -8053,10 +8064,10 @@
         <v>2016</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>48</v>
@@ -8075,7 +8086,7 @@
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>73</v>
@@ -8084,10 +8095,10 @@
         <v>2018</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>39</v>
@@ -8103,6 +8114,19 @@
         <v>28</v>
       </c>
       <c r="K200" s="2"/>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A201" s="3"/>
+      <c r="B201" s="3"/>
+      <c r="C201" s="3"/>
+      <c r="D201" s="3"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="3"/>
+      <c r="G201" s="3"/>
+      <c r="H201" s="3"/>
+      <c r="I201" s="3"/>
+      <c r="J201" s="3"/>
+      <c r="K201" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated the analysis files
</commit_message>
<xml_diff>
--- a/Overall Files/Analysis Result.xlsx
+++ b/Overall Files/Analysis Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minsik/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90690E6-0861-5B4A-9EA3-4BB2C0CEFEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9735835-1521-AE4A-8901-90BD460D9642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{D191EDB1-F553-D84A-B803-B27A1F8FBA75}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D191EDB1-F553-D84A-B803-B27A1F8FBA75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1743,11 +1743,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2062,10 +2061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78730E6-1DB0-FD44-93CC-339688788B9E}">
-  <dimension ref="A1:K201"/>
+  <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="G175" workbookViewId="0">
+      <selection activeCell="K200" sqref="A1:K200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6802,7 +6801,7 @@
         <v>377</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>40</v>
@@ -8115,19 +8114,6 @@
       </c>
       <c r="K200" s="2"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A201" s="3"/>
-      <c r="B201" s="3"/>
-      <c r="C201" s="3"/>
-      <c r="D201" s="3"/>
-      <c r="E201" s="3"/>
-      <c r="F201" s="3"/>
-      <c r="G201" s="3"/>
-      <c r="H201" s="3"/>
-      <c r="I201" s="3"/>
-      <c r="J201" s="3"/>
-      <c r="K201" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>